<commit_message>
Adição dos arquivos e os testes
</commit_message>
<xml_diff>
--- a/Material de Apoio/Caminhos.xlsx
+++ b/Material de Apoio/Caminhos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="46">
   <si>
     <t>Externo</t>
   </si>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,6 +207,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -214,7 +217,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -252,9 +255,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,9 +290,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,9 +342,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -500,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,6 +555,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -549,36 +587,96 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-1</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="1">
+        <v>-1</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-1</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="1">
+        <v>-1</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
@@ -587,14 +685,47 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-1</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -607,14 +738,32 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D8" s="1">
+        <v>-1</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B9" s="1">
+        <v>-1</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
@@ -623,6 +772,18 @@
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -638,6 +799,21 @@
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>-1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -646,8 +822,26 @@
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-1</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -657,11 +851,20 @@
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C12" s="1">
+        <v>-1</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-1</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>12</v>
@@ -677,30 +880,84 @@
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C13" s="1">
+        <v>-1</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-1</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F14" s="1">
+        <v>-1</v>
+      </c>
       <c r="G14" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="H14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-1</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E15" s="1">
+        <v>-1</v>
+      </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -738,17 +995,38 @@
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B19" s="1">
+        <v>-1</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D19" s="1">
+        <v>-1</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="F19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B20" s="1">
+        <v>-1</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
@@ -757,17 +1035,47 @@
       </c>
       <c r="E20" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="F20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B21" s="1">
+        <v>-1</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="E21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -777,6 +1085,21 @@
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-1</v>
+      </c>
       <c r="H22" s="1" t="s">
         <v>19</v>
       </c>
@@ -794,8 +1117,20 @@
       <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>-1</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="H23" s="1">
+        <v>-1</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>21</v>
@@ -811,17 +1146,41 @@
       <c r="C24" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>-1</v>
+      </c>
       <c r="F24" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G24" s="1">
+        <v>-1</v>
+      </c>
       <c r="H24" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="I24" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>-1</v>
+      </c>
       <c r="F25" s="1" t="s">
         <v>19</v>
       </c>
@@ -845,8 +1204,20 @@
       <c r="C26" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>-1</v>
+      </c>
       <c r="G26" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="H26" s="1">
+        <v>-1</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>24</v>
@@ -862,17 +1233,41 @@
       <c r="C27" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>-1</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="G27" s="1">
+        <v>-1</v>
+      </c>
       <c r="H27" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="I27" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>-1</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>22</v>
       </c>
@@ -896,8 +1291,20 @@
       <c r="C29" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="D29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>-1</v>
+      </c>
       <c r="G29" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="H29" s="1">
+        <v>-1</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>27</v>
@@ -913,17 +1320,41 @@
       <c r="C30" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="D30" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>-1</v>
+      </c>
       <c r="F30" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="G30" s="1">
+        <v>-1</v>
+      </c>
       <c r="H30" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="I30" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B31" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>-1</v>
+      </c>
       <c r="F31" s="1" t="s">
         <v>25</v>
       </c>
@@ -947,8 +1378,20 @@
       <c r="C32" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D32" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>-1</v>
+      </c>
       <c r="G32" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="H32" s="1">
+        <v>-1</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>30</v>
@@ -964,17 +1407,41 @@
       <c r="C33" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="D33" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>-1</v>
+      </c>
       <c r="F33" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="G33" s="1">
+        <v>-1</v>
+      </c>
       <c r="H33" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="I33" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B34" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C34" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>-1</v>
+      </c>
       <c r="F34" s="1" t="s">
         <v>28</v>
       </c>
@@ -998,8 +1465,20 @@
       <c r="C35" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="D35" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F35" s="1">
+        <v>-1</v>
+      </c>
       <c r="G35" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="H35" s="1">
+        <v>-1</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>33</v>
@@ -1015,17 +1494,41 @@
       <c r="C36" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="D36" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E36" s="1">
+        <v>-1</v>
+      </c>
       <c r="F36" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="G36" s="1">
+        <v>-1</v>
+      </c>
       <c r="H36" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="I36" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E37" s="1">
+        <v>-1</v>
+      </c>
       <c r="F37" s="1" t="s">
         <v>31</v>
       </c>
@@ -1046,11 +1549,26 @@
       <c r="B38" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="C38" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F38" s="1">
+        <v>-1</v>
+      </c>
       <c r="G38" s="1" t="s">
         <v>33</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="I38" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1060,8 +1578,23 @@
       <c r="B39" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C39" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>-1</v>
+      </c>
       <c r="F39" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="G39" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H39" s="1">
+        <v>-1</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>37</v>
@@ -1071,22 +1604,58 @@
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="B40" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C40" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>-1</v>
+      </c>
       <c r="E40" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="F40" s="1">
+        <v>-1</v>
+      </c>
       <c r="G40" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="H40" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I40" s="1">
+        <v>-1</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="B41" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>-1</v>
+      </c>
       <c r="D41" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="E41" s="1">
+        <v>-1</v>
+      </c>
       <c r="F41" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="G41" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H41" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I41" s="1">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>